<commit_message>
better airport pngs and TSA chart
</commit_message>
<xml_diff>
--- a/flights-data/lax_out.xlsx
+++ b/flights-data/lax_out.xlsx
@@ -549,7 +549,7 @@
         <v>-22</v>
       </c>
       <c r="G2">
-        <v>-2.52</v>
+        <v>-2.46</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -572,7 +572,7 @@
         <v>-32</v>
       </c>
       <c r="G3">
-        <v>-3.5</v>
+        <v>-3.38</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -595,7 +595,7 @@
         <v>-24</v>
       </c>
       <c r="G4">
-        <v>-2.7</v>
+        <v>-2.63</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -618,7 +618,7 @@
         <v>-20</v>
       </c>
       <c r="G5">
-        <v>-2.21</v>
+        <v>-2.16</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -641,7 +641,7 @@
         <v>-25</v>
       </c>
       <c r="G6">
-        <v>-2.74</v>
+        <v>-2.67</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -664,7 +664,7 @@
         <v>-15</v>
       </c>
       <c r="G7">
-        <v>-1.74</v>
+        <v>-1.71</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -687,7 +687,7 @@
         <v>-17</v>
       </c>
       <c r="G8">
-        <v>-2.09</v>
+        <v>-2.05</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -710,7 +710,7 @@
         <v>-33</v>
       </c>
       <c r="G9">
-        <v>-3.69</v>
+        <v>-3.56</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -733,7 +733,7 @@
         <v>-26</v>
       </c>
       <c r="G10">
-        <v>-2.88</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -756,7 +756,7 @@
         <v>-32</v>
       </c>
       <c r="G11">
-        <v>-3.56</v>
+        <v>-3.44</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -779,7 +779,7 @@
         <v>-36</v>
       </c>
       <c r="G12">
-        <v>-3.9</v>
+        <v>-3.75</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -802,7 +802,7 @@
         <v>-38</v>
       </c>
       <c r="G13">
-        <v>-4.12</v>
+        <v>-3.96</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -825,7 +825,7 @@
         <v>-34</v>
       </c>
       <c r="G14">
-        <v>-3.91</v>
+        <v>-3.76</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -848,7 +848,7 @@
         <v>-32</v>
       </c>
       <c r="G15">
-        <v>-3.86</v>
+        <v>-3.72</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -871,7 +871,7 @@
         <v>-32</v>
       </c>
       <c r="G16">
-        <v>-3.59</v>
+        <v>-3.46</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -894,7 +894,7 @@
         <v>-25</v>
       </c>
       <c r="G17">
-        <v>-2.81</v>
+        <v>-2.73</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -917,7 +917,7 @@
         <v>-31</v>
       </c>
       <c r="G18">
-        <v>-3.44</v>
+        <v>-3.33</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -940,7 +940,7 @@
         <v>-49</v>
       </c>
       <c r="G19">
-        <v>-5.3</v>
+        <v>-5.03</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -963,7 +963,7 @@
         <v>-37</v>
       </c>
       <c r="G20">
-        <v>-4.03</v>
+        <v>-3.87</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -986,7 +986,7 @@
         <v>-27</v>
       </c>
       <c r="G21">
-        <v>-3.11</v>
+        <v>-3.02</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1009,7 +1009,7 @@
         <v>-31</v>
       </c>
       <c r="G22">
-        <v>-3.51</v>
+        <v>-3.4</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1032,7 +1032,7 @@
         <v>-40</v>
       </c>
       <c r="G23">
-        <v>-4.52</v>
+        <v>-4.32</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1055,7 +1055,7 @@
         <v>-32</v>
       </c>
       <c r="G24">
-        <v>-3.58</v>
+        <v>-3.46</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1078,7 +1078,7 @@
         <v>-46</v>
       </c>
       <c r="G25">
-        <v>-5.14</v>
+        <v>-4.89</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1101,7 +1101,7 @@
         <v>-45</v>
       </c>
       <c r="G26">
-        <v>-4.93</v>
+        <v>-4.7</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1124,7 +1124,7 @@
         <v>-45</v>
       </c>
       <c r="G27">
-        <v>-4.8</v>
+        <v>-4.58</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1147,7 +1147,7 @@
         <v>-55</v>
       </c>
       <c r="G28">
-        <v>-6.29</v>
+        <v>-5.91</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1170,7 +1170,7 @@
         <v>-58</v>
       </c>
       <c r="G29">
-        <v>-6.91</v>
+        <v>-6.47</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1193,7 +1193,7 @@
         <v>-73</v>
       </c>
       <c r="G30">
-        <v>-8.24</v>
+        <v>-7.61</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1216,7 +1216,7 @@
         <v>-83</v>
       </c>
       <c r="G31">
-        <v>-9.58</v>
+        <v>-8.75</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1239,7 +1239,7 @@
         <v>-113</v>
       </c>
       <c r="G32">
-        <v>-13.93</v>
+        <v>-12.23</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1262,7 +1262,7 @@
         <v>-162</v>
       </c>
       <c r="G33">
-        <v>-20.05</v>
+        <v>-16.7</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1285,7 +1285,7 @@
         <v>-174</v>
       </c>
       <c r="G34">
-        <v>-22.28</v>
+        <v>-18.22</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1308,7 +1308,7 @@
         <v>-251</v>
       </c>
       <c r="G35">
-        <v>-37.35</v>
+        <v>-27.19</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1331,7 +1331,7 @@
         <v>-253</v>
       </c>
       <c r="G36">
-        <v>-40.81</v>
+        <v>-28.98</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1354,7 +1354,7 @@
         <v>-330</v>
       </c>
       <c r="G37">
-        <v>-56.03</v>
+        <v>-35.91</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1377,7 +1377,7 @@
         <v>-358</v>
       </c>
       <c r="G38">
-        <v>-63.36</v>
+        <v>-38.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>